<commit_message>
Added code for Tambah/Hapus Group User
as per summary
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/PROGRESS.xlsx
+++ b/_DOCUMENTS_/PROGRESS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
   <si>
     <t>Penerimaan Piutang</t>
   </si>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,6 +700,9 @@
       <c r="E6" t="s">
         <v>42</v>
       </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">

</xml_diff>

<commit_message>
Added code for Master Cabang
as per summary
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/PROGRESS.xlsx
+++ b/_DOCUMENTS_/PROGRESS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_PROJECT_\RoyalPetz\_DOCUMENTS_\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RoyalPetz\_DOCUMENTS_\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="101">
   <si>
     <t>Penerimaan Piutang</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>Change Password</t>
+  </si>
+  <si>
+    <t>Master Cabang</t>
   </si>
 </sst>
 </file>
@@ -1280,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C9" sqref="C9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,6 +1354,33 @@
         <v>42</v>
       </c>
     </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Master Kategori and Master Unit
as per summary
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/PROGRESS.xlsx
+++ b/_DOCUMENTS_/PROGRESS.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
   <si>
     <t>Penerimaan Piutang</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>SAVE TO DATABASE</t>
+  </si>
+  <si>
+    <t>Master Category</t>
   </si>
 </sst>
 </file>
@@ -1292,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,6 +1319,9 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
       <c r="D3" t="s">
         <v>94</v>
       </c>
@@ -1404,6 +1410,33 @@
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>